<commit_message>
new student management | download template | upload | add | delete
</commit_message>
<xml_diff>
--- a/DormManagement/Server/download/BedTemplate.xlsx
+++ b/DormManagement/Server/download/BedTemplate.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17927"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18067"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -408,7 +408,7 @@
   <dimension ref="A1:H1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
+      <selection activeCell="G1" sqref="G1:G1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -452,18 +452,21 @@
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
-  <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B1048576">
+  <dataValidations count="5">
+    <dataValidation type="textLength" operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="学号应为十位数字" sqref="G1:G1048576">
+      <formula1>10</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="楼号仅能输入5或13或14" sqref="B1:B1048576">
       <formula1>"5,13,14"</formula1>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="性别仅能输入“男”或“女”" sqref="E1:E1048576">
+      <formula1>"男,女"</formula1>
+    </dataValidation>
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="床位编号仅能输入数字" sqref="D1:D1048576">
       <formula1>1</formula1>
       <formula2>10</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E1048576">
-      <formula1>"男,女"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="状态仅能输入“已入住”，“已分配”或“空床”" sqref="F1:F1048576">
       <formula1>"已入住,已分配,空床"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>